<commit_message>
added duplicate conntent to xlx
</commit_message>
<xml_diff>
--- a/DuplicateMobileNumberList.xlsx
+++ b/DuplicateMobileNumberList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Mobile_No</t>
   </si>
@@ -83,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -113,12 +113,56 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>